<commit_message>
correcion AV-MCPS y MCPS
</commit_message>
<xml_diff>
--- a/codigo_final/final/prediccion_a_un_paso/analisis/Resultados_diferenciacion/resumen_estadistico_completo.xlsx
+++ b/codigo_final/final/prediccion_a_un_paso/analisis/Resultados_diferenciacion/resumen_estadistico_completo.xlsx
@@ -524,19 +524,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.15833986602997</v>
+        <v>1.130039812000503</v>
       </c>
       <c r="E3" t="n">
-        <v>1.336211969667334</v>
+        <v>1.275815659588881</v>
       </c>
       <c r="F3" t="n">
-        <v>0.585436068693754</v>
+        <v>0.5828155900050277</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2860775892003131</v>
+        <v>0.3008685073931974</v>
       </c>
       <c r="H3" t="n">
-        <v>49.45904169730034</v>
+        <v>48.42521619010283</v>
       </c>
     </row>
     <row r="4">
@@ -716,19 +716,19 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.091725471286789</v>
+        <v>1.191894586896629</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9334623646906376</v>
+        <v>1.514454092434213</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5644823138201085</v>
+        <v>0.5815323770219396</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2752410849618823</v>
+        <v>0.2874993982014941</v>
       </c>
       <c r="H9" t="n">
-        <v>48.29448165620177</v>
+        <v>51.20941202224161</v>
       </c>
     </row>
     <row r="10">
@@ -812,19 +812,19 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.820314378143563</v>
+        <v>1.772826884560276</v>
       </c>
       <c r="E12" t="n">
-        <v>1.698910232159862</v>
+        <v>1.874978778710598</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5938249516279056</v>
+        <v>0.6130081529339334</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3087028436001204</v>
+        <v>0.3241854572552367</v>
       </c>
       <c r="H12" t="n">
-        <v>67.3778903931136</v>
+        <v>65.42199589408973</v>
       </c>
     </row>
     <row r="13">
@@ -1004,19 +1004,19 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1.764131099751633</v>
+        <v>1.870968211745923</v>
       </c>
       <c r="E18" t="n">
-        <v>1.633401654481311</v>
+        <v>1.698016838090766</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6055624718902791</v>
+        <v>0.6183860409444772</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3187160842366211</v>
+        <v>0.3289204103846034</v>
       </c>
       <c r="H18" t="n">
-        <v>65.67361280714714</v>
+        <v>66.948340593803</v>
       </c>
     </row>
     <row r="19">
@@ -1100,19 +1100,19 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1.172283448247199</v>
+        <v>1.042393725434717</v>
       </c>
       <c r="E21" t="n">
-        <v>1.213988037774737</v>
+        <v>0.8462652785780268</v>
       </c>
       <c r="F21" t="n">
-        <v>0.588842985293191</v>
+        <v>0.5994023930984035</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2885310159134679</v>
+        <v>0.2927460172055956</v>
       </c>
       <c r="H21" t="n">
-        <v>49.76957269390518</v>
+        <v>42.49750564754882</v>
       </c>
     </row>
     <row r="22">
@@ -1292,19 +1292,19 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.332696299862324</v>
+        <v>1.359591281829325</v>
       </c>
       <c r="E27" t="n">
-        <v>1.365900733818041</v>
+        <v>1.429551824566111</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5929401248181848</v>
+        <v>0.5965042334550942</v>
       </c>
       <c r="G27" t="n">
-        <v>0.281024286278975</v>
+        <v>0.2796140497361679</v>
       </c>
       <c r="H27" t="n">
-        <v>55.50823358034091</v>
+        <v>56.12620929339146</v>
       </c>
     </row>
     <row r="28">
@@ -1388,19 +1388,19 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1.023621315158779</v>
+        <v>0.9524985194888282</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8128573203629967</v>
+        <v>0.6690640918403911</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6068246806595237</v>
+        <v>0.6078029594341335</v>
       </c>
       <c r="G30" t="n">
-        <v>0.3325620963467214</v>
+        <v>0.3307531955687637</v>
       </c>
       <c r="H30" t="n">
-        <v>40.71785418366402</v>
+        <v>36.18856649138735</v>
       </c>
     </row>
     <row r="31">
@@ -1580,19 +1580,19 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.022860757388425</v>
+        <v>0.9606868561418768</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8261089312922864</v>
+        <v>0.6952218388957947</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6059918055615643</v>
+        <v>0.5980650900149307</v>
       </c>
       <c r="G36" t="n">
-        <v>0.3060207813805415</v>
+        <v>0.3069677239599218</v>
       </c>
       <c r="H36" t="n">
-        <v>40.75520043326456</v>
+        <v>37.74609424586456</v>
       </c>
     </row>
     <row r="37">
@@ -1676,19 +1676,19 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.328554823685909</v>
+        <v>1.08073914074972</v>
       </c>
       <c r="E39" t="n">
-        <v>1.399521400665189</v>
+        <v>0.9193874723821164</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6081741146463447</v>
+        <v>0.5922852545941724</v>
       </c>
       <c r="G39" t="n">
-        <v>0.3312239714370764</v>
+        <v>0.3049061961032624</v>
       </c>
       <c r="H39" t="n">
-        <v>54.22288160009521</v>
+        <v>45.19627981796808</v>
       </c>
     </row>
     <row r="40">
@@ -1868,19 +1868,19 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.647721781287249</v>
+        <v>1.65160584235895</v>
       </c>
       <c r="E45" t="n">
-        <v>2.293201811662968</v>
+        <v>2.304315262760082</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5887324263708575</v>
+        <v>0.5997523877657435</v>
       </c>
       <c r="G45" t="n">
-        <v>0.3077507943063949</v>
+        <v>0.3307587595548684</v>
       </c>
       <c r="H45" t="n">
-        <v>64.26991297578635</v>
+        <v>63.68671190281506</v>
       </c>
     </row>
     <row r="46">
@@ -1964,19 +1964,19 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.36155129095691</v>
+        <v>1.888207575285985</v>
       </c>
       <c r="E48" t="n">
-        <v>3.264379658547925</v>
+        <v>1.974674218246942</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6349968520357645</v>
+        <v>0.6484752350963774</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3822758573018297</v>
+        <v>0.42350447091781</v>
       </c>
       <c r="H48" t="n">
-        <v>73.11102856552985</v>
+        <v>65.65657062369532</v>
       </c>
     </row>
     <row r="49">
@@ -2156,19 +2156,19 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2.589638934553707</v>
+        <v>2.615182453893337</v>
       </c>
       <c r="E54" t="n">
-        <v>2.925083577111379</v>
+        <v>3.038460580965362</v>
       </c>
       <c r="F54" t="n">
-        <v>0.6404991227894723</v>
+        <v>0.6438414075788274</v>
       </c>
       <c r="G54" t="n">
-        <v>0.3744023481548663</v>
+        <v>0.363440656298077</v>
       </c>
       <c r="H54" t="n">
-        <v>75.26685615344849</v>
+        <v>75.38063141176585</v>
       </c>
     </row>
     <row r="55">
@@ -2252,19 +2252,19 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>6.249799140020401</v>
+        <v>6.461767059647445</v>
       </c>
       <c r="E57" t="n">
-        <v>11.19549906115284</v>
+        <v>11.63974795365123</v>
       </c>
       <c r="F57" t="n">
-        <v>0.6362873243014681</v>
+        <v>0.6574101129956289</v>
       </c>
       <c r="G57" t="n">
-        <v>0.3582925155567679</v>
+        <v>0.3861310167055895</v>
       </c>
       <c r="H57" t="n">
-        <v>89.81907562073441</v>
+        <v>89.8261558034019</v>
       </c>
     </row>
     <row r="58">
@@ -2444,19 +2444,19 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>8.387917820273689</v>
+        <v>8.143928040651026</v>
       </c>
       <c r="E63" t="n">
-        <v>11.15418778105534</v>
+        <v>11.29908971185616</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6386562645594155</v>
+        <v>0.6468857169367002</v>
       </c>
       <c r="G63" t="n">
-        <v>0.3422706900172273</v>
+        <v>0.3843845969905713</v>
       </c>
       <c r="H63" t="n">
-        <v>92.38599759506732</v>
+        <v>92.05683407677816</v>
       </c>
     </row>
     <row r="64">
@@ -2540,19 +2540,19 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>3.674304911046021</v>
+        <v>3.429714268763714</v>
       </c>
       <c r="E66" t="n">
-        <v>9.806844951884017</v>
+        <v>10.09286962487652</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6219063729426846</v>
+        <v>0.6318799426006594</v>
       </c>
       <c r="G66" t="n">
-        <v>0.351259656468622</v>
+        <v>0.3825753437712935</v>
       </c>
       <c r="H66" t="n">
-        <v>83.07417625921423</v>
+        <v>81.57630947990228</v>
       </c>
     </row>
     <row r="67">
@@ -2732,19 +2732,19 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>4.028608957775186</v>
+        <v>4.197278605559789</v>
       </c>
       <c r="E72" t="n">
-        <v>9.229928439902128</v>
+        <v>9.341076041519006</v>
       </c>
       <c r="F72" t="n">
-        <v>0.6361703637156554</v>
+        <v>0.6395557151125862</v>
       </c>
       <c r="G72" t="n">
-        <v>0.3621576151234229</v>
+        <v>0.3621176375219149</v>
       </c>
       <c r="H72" t="n">
-        <v>84.20868417899308</v>
+        <v>84.76260989047952</v>
       </c>
     </row>
     <row r="73">
@@ -2828,19 +2828,19 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1.892911664764399</v>
+        <v>2.020363954587721</v>
       </c>
       <c r="E75" t="n">
-        <v>2.087525958242063</v>
+        <v>2.293811255464086</v>
       </c>
       <c r="F75" t="n">
-        <v>0.6109490516701191</v>
+        <v>0.6252891778139488</v>
       </c>
       <c r="G75" t="n">
-        <v>0.3055783649170291</v>
+        <v>0.3170081591871743</v>
       </c>
       <c r="H75" t="n">
-        <v>67.72437599478997</v>
+        <v>69.05066652005547</v>
       </c>
     </row>
     <row r="76">
@@ -3020,19 +3020,19 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>2.464186319395024</v>
+        <v>2.351628933613348</v>
       </c>
       <c r="E81" t="n">
-        <v>3.341040452170607</v>
+        <v>3.248806248950661</v>
       </c>
       <c r="F81" t="n">
-        <v>0.6204593580173743</v>
+        <v>0.6225967702997584</v>
       </c>
       <c r="G81" t="n">
-        <v>0.2941472114279274</v>
+        <v>0.2984945226681516</v>
       </c>
       <c r="H81" t="n">
-        <v>74.8209235180844</v>
+        <v>73.52487199827399</v>
       </c>
     </row>
     <row r="82">
@@ -3116,19 +3116,19 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2.030324681559674</v>
+        <v>1.773589740420534</v>
       </c>
       <c r="E84" t="n">
-        <v>2.598943552961664</v>
+        <v>2.061381867598989</v>
       </c>
       <c r="F84" t="n">
-        <v>0.5744826727926071</v>
+        <v>0.5771293380505662</v>
       </c>
       <c r="G84" t="n">
-        <v>0.3117182146082071</v>
+        <v>0.3016652662707829</v>
       </c>
       <c r="H84" t="n">
-        <v>71.70488651345678</v>
+        <v>67.45981751598747</v>
       </c>
     </row>
     <row r="85">
@@ -3308,19 +3308,19 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>2.417435335734541</v>
+        <v>2.385951200020108</v>
       </c>
       <c r="E90" t="n">
-        <v>2.880926244443793</v>
+        <v>2.925001836010356</v>
       </c>
       <c r="F90" t="n">
-        <v>0.5586229598503741</v>
+        <v>0.5643341557464877</v>
       </c>
       <c r="G90" t="n">
-        <v>0.288539364315775</v>
+        <v>0.2961576268678773</v>
       </c>
       <c r="H90" t="n">
-        <v>76.89191716556772</v>
+        <v>76.34762371746196</v>
       </c>
     </row>
     <row r="91">
@@ -3404,19 +3404,19 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>1.540036781680823</v>
+        <v>1.537512660735602</v>
       </c>
       <c r="E93" t="n">
-        <v>1.531243727888035</v>
+        <v>1.857977131638517</v>
       </c>
       <c r="F93" t="n">
-        <v>0.6009087972872281</v>
+        <v>0.5975810084176308</v>
       </c>
       <c r="G93" t="n">
-        <v>0.3181154228406267</v>
+        <v>0.3327908348066964</v>
       </c>
       <c r="H93" t="n">
-        <v>60.98088016888883</v>
+        <v>61.13326259494172</v>
       </c>
     </row>
     <row r="94">
@@ -3596,19 +3596,19 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>1.650271878594977</v>
+        <v>1.679638470195038</v>
       </c>
       <c r="E99" t="n">
-        <v>1.769486027325652</v>
+        <v>1.925028804510991</v>
       </c>
       <c r="F99" t="n">
-        <v>0.5894699844827302</v>
+        <v>0.5931741671016955</v>
       </c>
       <c r="G99" t="n">
-        <v>0.3188757763556272</v>
+        <v>0.3149634942528675</v>
       </c>
       <c r="H99" t="n">
-        <v>64.28043208343351</v>
+        <v>64.68441407913117</v>
       </c>
     </row>
     <row r="100">
@@ -3692,19 +3692,19 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>1.658467862551032</v>
+        <v>1.473442744897767</v>
       </c>
       <c r="E102" t="n">
-        <v>2.374964744078377</v>
+        <v>2.024984761337615</v>
       </c>
       <c r="F102" t="n">
-        <v>0.6306009462058975</v>
+        <v>0.6404060318012496</v>
       </c>
       <c r="G102" t="n">
-        <v>0.3525331246335518</v>
+        <v>0.3634850751511958</v>
       </c>
       <c r="H102" t="n">
-        <v>61.97689684285375</v>
+        <v>56.53675488790824</v>
       </c>
     </row>
     <row r="103">
@@ -3884,19 +3884,19 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>2.179991911645855</v>
+        <v>2.095400843123908</v>
       </c>
       <c r="E108" t="n">
-        <v>4.663977928976091</v>
+        <v>4.545415804976174</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6216091409409242</v>
+        <v>0.6410300872521241</v>
       </c>
       <c r="G108" t="n">
-        <v>0.3132201237345626</v>
+        <v>0.3587792290280774</v>
       </c>
       <c r="H108" t="n">
-        <v>71.48571342764201</v>
+        <v>69.40775845558741</v>
       </c>
     </row>
     <row r="109">
@@ -3980,19 +3980,19 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0.8409993926738577</v>
+        <v>0.9172207748045611</v>
       </c>
       <c r="E111" t="n">
-        <v>1.028753899941465</v>
+        <v>1.310887195018372</v>
       </c>
       <c r="F111" t="n">
-        <v>0.2762123957926001</v>
+        <v>0.2834395874701757</v>
       </c>
       <c r="G111" t="n">
-        <v>0.04338911480321651</v>
+        <v>0.06613406133916325</v>
       </c>
       <c r="H111" t="n">
-        <v>67.15664741273883</v>
+        <v>69.09799742264121</v>
       </c>
     </row>
     <row r="112">
@@ -4172,19 +4172,19 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>1.005645315373894</v>
+        <v>1.004358600562757</v>
       </c>
       <c r="E117" t="n">
-        <v>1.54388593696543</v>
+        <v>1.54588599717618</v>
       </c>
       <c r="F117" t="n">
-        <v>0.2807648072865274</v>
+        <v>0.2811652669671177</v>
       </c>
       <c r="G117" t="n">
-        <v>0.05433178754993106</v>
+        <v>0.04729203065788602</v>
       </c>
       <c r="H117" t="n">
-        <v>72.08113009683335</v>
+        <v>72.00549018950238</v>
       </c>
     </row>
     <row r="118">
@@ -4268,19 +4268,19 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>1.556377485696372</v>
+        <v>1.486337451856089</v>
       </c>
       <c r="E120" t="n">
-        <v>1.854392206025991</v>
+        <v>1.678731597409714</v>
       </c>
       <c r="F120" t="n">
-        <v>0.4370056485310811</v>
+        <v>0.4440790461361111</v>
       </c>
       <c r="G120" t="n">
-        <v>0.07983128812995791</v>
+        <v>0.08247294571698363</v>
       </c>
       <c r="H120" t="n">
-        <v>71.92161589670188</v>
+        <v>70.1225959433667</v>
       </c>
     </row>
     <row r="121">
@@ -4460,19 +4460,19 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>2.024628331454544</v>
+        <v>2.068229170699706</v>
       </c>
       <c r="E126" t="n">
-        <v>3.247477115166079</v>
+        <v>3.319685289326045</v>
       </c>
       <c r="F126" t="n">
-        <v>0.4452071156090608</v>
+        <v>0.4485041848075516</v>
       </c>
       <c r="G126" t="n">
-        <v>0.08634525362273264</v>
+        <v>0.09482021137006048</v>
       </c>
       <c r="H126" t="n">
-        <v>78.01042746007546</v>
+        <v>78.31457987531346</v>
       </c>
     </row>
     <row r="127">
@@ -4556,19 +4556,19 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>1.887095816730686</v>
+        <v>1.81890260086058</v>
       </c>
       <c r="E129" t="n">
-        <v>2.159622898992734</v>
+        <v>2.236590111403163</v>
       </c>
       <c r="F129" t="n">
-        <v>0.6225196574718871</v>
+        <v>0.6133713213769625</v>
       </c>
       <c r="G129" t="n">
-        <v>0.1049157356886284</v>
+        <v>0.1034113914285109</v>
       </c>
       <c r="H129" t="n">
-        <v>67.01176209746592</v>
+        <v>66.2779457741851</v>
       </c>
     </row>
     <row r="130">
@@ -4748,19 +4748,19 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>2.13517929311569</v>
+        <v>2.115623043598457</v>
       </c>
       <c r="E135" t="n">
-        <v>2.92315379037992</v>
+        <v>3.039212066584865</v>
       </c>
       <c r="F135" t="n">
-        <v>0.6242253660932638</v>
+        <v>0.6292179154746675</v>
       </c>
       <c r="G135" t="n">
-        <v>0.1162116155960376</v>
+        <v>0.1117324142731587</v>
       </c>
       <c r="H135" t="n">
-        <v>70.76473305516262</v>
+        <v>70.25850529570558</v>
       </c>
     </row>
     <row r="136">
@@ -4844,19 +4844,19 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>4.352364026180645</v>
+        <v>3.96523786800304</v>
       </c>
       <c r="E138" t="n">
-        <v>8.859170871798316</v>
+        <v>9.074306383649709</v>
       </c>
       <c r="F138" t="n">
-        <v>1.095340570923261</v>
+        <v>1.116938443963994</v>
       </c>
       <c r="G138" t="n">
-        <v>0.1916715263822192</v>
+        <v>0.2320419365983491</v>
       </c>
       <c r="H138" t="n">
-        <v>74.83343386870925</v>
+        <v>71.83174172281112</v>
       </c>
     </row>
     <row r="139">
@@ -5036,19 +5036,19 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>5.026942582572339</v>
+        <v>4.979707627148833</v>
       </c>
       <c r="E144" t="n">
-        <v>8.701340906458455</v>
+        <v>8.730470938522354</v>
       </c>
       <c r="F144" t="n">
-        <v>1.070868156616795</v>
+        <v>1.089665349160785</v>
       </c>
       <c r="G144" t="n">
-        <v>0.1780579514396816</v>
+        <v>0.2093026209643546</v>
       </c>
       <c r="H144" t="n">
-        <v>78.69742613871631</v>
+        <v>78.11788500955265</v>
       </c>
     </row>
     <row r="145">

</xml_diff>